<commit_message>
mark up TB und MF
</commit_message>
<xml_diff>
--- a/docs/Baernreither_Personenregister_2023.xlsx
+++ b/docs/Baernreither_Personenregister_2023.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2d7251a833aeb89d/Dokumente/BAERNREITHER 2023/Baernreither CLARIAH 2022/Editionsdateien für CLARIAH/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christofaichner/Documents/GitHub/baernreither-data/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="199" documentId="8_{EBB89A8C-4913-4638-BCE7-70A9C2F10EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43BECEFA-7620-4308-997C-B6256CEF4F16}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13880"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,18 +19,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="941">
   <si>
     <t>Abrahamowicz</t>
   </si>
@@ -2440,7 +2439,6 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>ant</t>
@@ -2953,12 +2951,30 @@
       <t>) u. 1907-1908 1. Vizepräs. öAH, 1887-1918 MmährLt, 9.11.1908-30.10.1909 österr. Minister o.P. (Tschech. Landsmannminister), 1912-1918 MöHH (Gruppe der Rechten)</t>
     </r>
   </si>
+  <si>
+    <t>Kaljajew</t>
+  </si>
+  <si>
+    <t>&lt;persName key="KaljajewIwan" ref="https://d-nb.info/gnd/120011468"&gt;</t>
+  </si>
+  <si>
+    <t>Iwan Platonowitsch</t>
+  </si>
+  <si>
+    <t>Sozialrevolutionär</t>
+  </si>
+  <si>
+    <t>https://d-nb.info/gnd/120011468</t>
+  </si>
+  <si>
+    <t>KaljajewIwan</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3016,13 +3032,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3137,7 +3146,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3262,10 +3271,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -3643,18 +3655,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:J156" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:J157" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nachname" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Spalte1" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Namenszusatz" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Vorname" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Geburtsjahr" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Sterbejahr" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Bezeichnung" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="GND" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Keywert" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Varianten" dataDxfId="0"/>
+    <tableColumn id="1" name="Nachname" dataDxfId="9"/>
+    <tableColumn id="11" name="Spalte1" dataDxfId="8"/>
+    <tableColumn id="2" name="Namenszusatz" dataDxfId="7"/>
+    <tableColumn id="3" name="Vorname" dataDxfId="6"/>
+    <tableColumn id="4" name="Geburtsjahr" dataDxfId="5"/>
+    <tableColumn id="5" name="Sterbejahr" dataDxfId="4"/>
+    <tableColumn id="6" name="Bezeichnung" dataDxfId="3"/>
+    <tableColumn id="7" name="GND" dataDxfId="2"/>
+    <tableColumn id="8" name="Keywert" dataDxfId="1"/>
+    <tableColumn id="9" name="Varianten" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3922,28 +3934,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J156"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B151" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D154" sqref="D154"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="66.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="6" max="6" width="7.5" customWidth="1"/>
     <col min="7" max="7" width="41" customWidth="1"/>
-    <col min="8" max="8" width="34.44140625" customWidth="1"/>
-    <col min="9" max="9" width="18.5546875" customWidth="1"/>
+    <col min="8" max="8" width="34.5" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>304</v>
       </c>
@@ -3975,7 +3987,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3987,7 +3999,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -4017,7 +4029,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -4047,7 +4059,7 @@
       </c>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -4077,7 +4089,7 @@
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -4107,7 +4119,7 @@
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -4137,7 +4149,7 @@
       </c>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>783</v>
       </c>
@@ -4167,7 +4179,7 @@
       </c>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>607</v>
       </c>
@@ -4197,7 +4209,7 @@
       </c>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>617</v>
       </c>
@@ -4227,7 +4239,7 @@
       </c>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="90" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>612</v>
       </c>
@@ -4255,7 +4267,7 @@
       </c>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>646</v>
       </c>
@@ -4285,7 +4297,7 @@
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>641</v>
       </c>
@@ -4313,7 +4325,7 @@
       </c>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="34" t="s">
         <v>786</v>
       </c>
@@ -4343,7 +4355,7 @@
       </c>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>602</v>
       </c>
@@ -4373,7 +4385,7 @@
       </c>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>785</v>
       </c>
@@ -4390,7 +4402,7 @@
       </c>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>594</v>
       </c>
@@ -4420,7 +4432,7 @@
       </c>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>781</v>
       </c>
@@ -4450,7 +4462,7 @@
       </c>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>580</v>
       </c>
@@ -4478,7 +4490,7 @@
       </c>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>784</v>
       </c>
@@ -4508,7 +4520,7 @@
       </c>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -4538,7 +4550,7 @@
       </c>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
@@ -4568,7 +4580,7 @@
       </c>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
@@ -4598,7 +4610,7 @@
       </c>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
@@ -4630,7 +4642,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
@@ -4660,7 +4672,7 @@
       </c>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>35</v>
       </c>
@@ -4690,7 +4702,7 @@
       </c>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>39</v>
       </c>
@@ -4720,7 +4732,7 @@
       </c>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>42</v>
       </c>
@@ -4752,7 +4764,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>45</v>
       </c>
@@ -4784,7 +4796,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>48</v>
       </c>
@@ -4814,7 +4826,7 @@
       </c>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>49</v>
       </c>
@@ -4844,7 +4856,7 @@
       </c>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" s="36" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="35" t="s">
         <v>807</v>
       </c>
@@ -4871,7 +4883,7 @@
       </c>
       <c r="J32" s="35"/>
     </row>
-    <row r="33" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
@@ -4901,7 +4913,7 @@
       </c>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>54</v>
       </c>
@@ -4931,7 +4943,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>58</v>
       </c>
@@ -4961,7 +4973,7 @@
       </c>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>61</v>
       </c>
@@ -4991,7 +5003,7 @@
       </c>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>64</v>
       </c>
@@ -5021,7 +5033,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>637</v>
       </c>
@@ -5046,7 +5058,7 @@
       </c>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>68</v>
       </c>
@@ -5078,7 +5090,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>72</v>
       </c>
@@ -5108,7 +5120,7 @@
       </c>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>74</v>
       </c>
@@ -5138,7 +5150,7 @@
       </c>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>76</v>
       </c>
@@ -5160,7 +5172,7 @@
       </c>
       <c r="J42" s="11"/>
     </row>
-    <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>78</v>
       </c>
@@ -5190,7 +5202,7 @@
       </c>
       <c r="J43" s="11"/>
     </row>
-    <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>79</v>
       </c>
@@ -5220,7 +5232,7 @@
       </c>
       <c r="J44" s="11"/>
     </row>
-    <row r="45" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
         <v>83</v>
       </c>
@@ -5252,7 +5264,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A46" s="14" t="s">
         <v>86</v>
       </c>
@@ -5282,7 +5294,7 @@
       </c>
       <c r="J46" s="16"/>
     </row>
-    <row r="47" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="105" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>88</v>
       </c>
@@ -5312,7 +5324,7 @@
       </c>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
         <v>813</v>
@@ -5331,7 +5343,7 @@
       </c>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>91</v>
       </c>
@@ -5357,7 +5369,7 @@
       </c>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>628</v>
       </c>
@@ -5387,7 +5399,7 @@
       </c>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>94</v>
       </c>
@@ -5419,7 +5431,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>97</v>
       </c>
@@ -5451,7 +5463,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>99</v>
       </c>
@@ -5483,7 +5495,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>102</v>
       </c>
@@ -5511,7 +5523,7 @@
       </c>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>514</v>
       </c>
@@ -5539,7 +5551,7 @@
       </c>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>514</v>
       </c>
@@ -5567,7 +5579,7 @@
       </c>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>782</v>
       </c>
@@ -5597,7 +5609,7 @@
       </c>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>632</v>
       </c>
@@ -5627,7 +5639,7 @@
       </c>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>105</v>
       </c>
@@ -5657,7 +5669,7 @@
       </c>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>107</v>
       </c>
@@ -5687,7 +5699,7 @@
       </c>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>110</v>
       </c>
@@ -5717,7 +5729,7 @@
       </c>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>114</v>
       </c>
@@ -5745,7 +5757,7 @@
       </c>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A63" s="38" t="s">
         <v>589</v>
       </c>
@@ -5775,7 +5787,7 @@
       </c>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A64" s="38" t="s">
         <v>598</v>
       </c>
@@ -5805,7 +5817,7 @@
       </c>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" ht="105" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>116</v>
       </c>
@@ -5835,7 +5847,7 @@
       </c>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>119</v>
       </c>
@@ -5863,7 +5875,7 @@
       </c>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
         <v>121</v>
       </c>
@@ -5895,7 +5907,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A68" s="12" t="s">
         <v>124</v>
       </c>
@@ -5923,7 +5935,7 @@
       </c>
       <c r="J68" s="11"/>
     </row>
-    <row r="69" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A69" s="14" t="s">
         <v>125</v>
       </c>
@@ -5951,2544 +5963,2572 @@
       </c>
       <c r="J69" s="16"/>
     </row>
-    <row r="70" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="3" t="s">
+    <row r="70" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A70" s="46" t="s">
+        <v>935</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>936</v>
+      </c>
+      <c r="C70" s="46"/>
+      <c r="D70" s="46" t="s">
+        <v>937</v>
+      </c>
+      <c r="E70" s="46">
+        <v>1877</v>
+      </c>
+      <c r="F70" s="46">
+        <v>1905</v>
+      </c>
+      <c r="G70" s="46" t="s">
+        <v>938</v>
+      </c>
+      <c r="H70" t="s">
+        <v>939</v>
+      </c>
+      <c r="I70" s="46" t="s">
+        <v>940</v>
+      </c>
+      <c r="J70" s="46"/>
+    </row>
+    <row r="71" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>699</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="E70" s="2">
+      <c r="E71" s="2">
         <v>1842</v>
       </c>
-      <c r="F70" s="2">
+      <c r="F71" s="2">
         <v>1916</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>877</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H71" t="s">
         <v>574</v>
       </c>
-      <c r="I70" s="2" t="s">
+      <c r="I71" s="2" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="3" t="s">
+    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>700</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E71" s="2">
+      <c r="E72" s="2">
         <v>1856</v>
       </c>
-      <c r="F71" s="2">
+      <c r="F72" s="2">
         <v>1945</v>
       </c>
-      <c r="G71" s="2" t="s">
+      <c r="G72" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="H71" t="s">
+      <c r="H72" t="s">
         <v>575</v>
       </c>
-      <c r="I71" s="2" t="s">
+      <c r="I72" s="2" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
+    <row r="73" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>701</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E72" s="2">
-        <v>1852</v>
-      </c>
-      <c r="F72" s="2">
-        <v>1911</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>878</v>
-      </c>
-      <c r="H72" s="2"/>
-      <c r="I72" s="2" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>702</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D73" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E73" s="2">
+        <v>1852</v>
+      </c>
+      <c r="F73" s="2">
+        <v>1911</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E74" s="2">
         <v>1847</v>
       </c>
-      <c r="F73" s="2">
+      <c r="F74" s="2">
         <v>1923</v>
       </c>
-      <c r="G73" s="2" t="s">
+      <c r="G74" s="2" t="s">
         <v>879</v>
       </c>
-      <c r="H73" t="s">
+      <c r="H74" t="s">
         <v>576</v>
       </c>
-      <c r="I73" s="2" t="s">
+      <c r="I74" s="2" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2" t="s">
+      <c r="C75" s="2"/>
+      <c r="D75" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="E74" s="2">
+      <c r="E75" s="2">
         <v>1854</v>
       </c>
-      <c r="F74" s="2">
+      <c r="F75" s="2">
         <v>1912</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="G75" s="2" t="s">
         <v>880</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H75" t="s">
         <v>577</v>
       </c>
-      <c r="I74" s="2" t="s">
+      <c r="I75" s="2" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
+    <row r="76" spans="1:10" ht="105" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>704</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="E75" s="2">
+      <c r="E76" s="2">
         <v>1850</v>
       </c>
-      <c r="F75" s="2">
+      <c r="F76" s="2">
         <v>1919</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="G76" s="2" t="s">
         <v>881</v>
       </c>
-      <c r="H75" s="1" t="s">
+      <c r="H76" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="I75" s="2" t="s">
+      <c r="I76" s="2" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
+    <row r="77" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>705</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="E76" s="2">
+      <c r="E77" s="2">
         <v>1852</v>
       </c>
-      <c r="F76" s="2">
+      <c r="F77" s="2">
         <v>1910</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="G77" s="2" t="s">
         <v>882</v>
       </c>
-      <c r="H76" t="s">
+      <c r="H77" t="s">
         <v>578</v>
       </c>
-      <c r="I76" s="2" t="s">
+      <c r="I77" s="2" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
+    <row r="78" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>706</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E77" s="2">
+      <c r="E78" s="2">
         <v>1837</v>
       </c>
-      <c r="F77" s="2">
+      <c r="F78" s="2">
         <v>1914</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="G78" s="2" t="s">
         <v>883</v>
       </c>
-      <c r="H77" t="s">
+      <c r="H78" t="s">
         <v>579</v>
       </c>
-      <c r="I77" s="2" t="s">
+      <c r="I78" s="2" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A78" s="12" t="s">
+    <row r="79" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A79" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>707</v>
       </c>
-      <c r="C78" s="13" t="s">
+      <c r="C79" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="D78" s="13" t="s">
+      <c r="D79" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E78" s="13">
+      <c r="E79" s="13">
         <v>1852</v>
       </c>
-      <c r="F78" s="13">
+      <c r="F79" s="13">
         <v>1909</v>
       </c>
-      <c r="G78" s="13" t="s">
+      <c r="G79" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="H78" t="s">
+      <c r="H79" t="s">
         <v>362</v>
       </c>
-      <c r="I78" s="13" t="s">
+      <c r="I79" s="13" t="s">
         <v>507</v>
       </c>
-      <c r="J78" s="11"/>
-    </row>
-    <row r="79" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A79" s="12" t="s">
+      <c r="J79" s="11"/>
+    </row>
+    <row r="80" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A80" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>708</v>
       </c>
-      <c r="C79" s="13" t="s">
+      <c r="C80" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D79" s="13" t="s">
+      <c r="D80" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="E79" s="13">
+      <c r="E80" s="13">
         <v>1856</v>
       </c>
-      <c r="F79" s="13">
+      <c r="F80" s="13">
         <v>1919</v>
       </c>
-      <c r="G79" s="13" t="s">
+      <c r="G80" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="H79" t="s">
+      <c r="H80" t="s">
         <v>363</v>
       </c>
-      <c r="I79" s="13" t="s">
+      <c r="I80" s="13" t="s">
         <v>506</v>
       </c>
-      <c r="J79" s="11"/>
-    </row>
-    <row r="80" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A80" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>709</v>
-      </c>
-      <c r="C80" s="13"/>
-      <c r="D80" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="E80" s="13">
-        <v>1841</v>
-      </c>
-      <c r="F80" s="13">
-        <v>1914</v>
-      </c>
-      <c r="G80" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="H80" t="s">
-        <v>364</v>
-      </c>
-      <c r="I80" s="13" t="s">
-        <v>505</v>
-      </c>
       <c r="J80" s="11"/>
     </row>
-    <row r="81" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A81" s="12" t="s">
         <v>135</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C81" s="13"/>
       <c r="D81" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E81" s="13">
+        <v>1841</v>
+      </c>
+      <c r="F81" s="13">
+        <v>1914</v>
+      </c>
+      <c r="G81" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="H81" t="s">
+        <v>364</v>
+      </c>
+      <c r="I81" s="13" t="s">
+        <v>505</v>
+      </c>
+      <c r="J81" s="11"/>
+    </row>
+    <row r="82" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A82" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="E81" s="13">
+      <c r="E82" s="13">
         <v>1802</v>
       </c>
-      <c r="F81" s="13">
+      <c r="F82" s="13">
         <v>1894</v>
       </c>
-      <c r="G81" s="13" t="s">
+      <c r="G82" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H82" t="s">
         <v>365</v>
       </c>
-      <c r="I81" s="13" t="s">
+      <c r="I82" s="13" t="s">
         <v>504</v>
       </c>
-      <c r="J81" s="11"/>
-    </row>
-    <row r="82" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A82" s="12" t="s">
+      <c r="J82" s="11"/>
+    </row>
+    <row r="83" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+      <c r="A83" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>711</v>
       </c>
-      <c r="C82" s="13" t="s">
+      <c r="C83" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D82" s="13" t="s">
+      <c r="D83" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="E82" s="13">
+      <c r="E83" s="13">
         <v>1860</v>
       </c>
-      <c r="F82" s="13">
+      <c r="F83" s="13">
         <v>1937</v>
       </c>
-      <c r="G82" s="13" t="s">
+      <c r="G83" s="13" t="s">
         <v>884</v>
       </c>
-      <c r="H82" t="s">
+      <c r="H83" t="s">
         <v>366</v>
       </c>
-      <c r="I82" s="13" t="s">
+      <c r="I83" s="13" t="s">
         <v>531</v>
       </c>
-      <c r="J82" s="11"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A83" s="12" t="s">
+      <c r="J83" s="11"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="C83" s="13" t="s">
+      <c r="C84" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="D83" s="13" t="s">
+      <c r="D84" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="E83" s="13">
+      <c r="E84" s="13">
         <v>1857</v>
       </c>
-      <c r="F83" s="13">
+      <c r="F84" s="13">
         <v>1928</v>
       </c>
-      <c r="G83" s="13" t="s">
+      <c r="G84" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="H83" t="s">
+      <c r="H84" t="s">
         <v>368</v>
       </c>
-      <c r="I83" s="13" t="s">
+      <c r="I84" s="13" t="s">
         <v>532</v>
       </c>
-      <c r="J83" s="11"/>
-    </row>
-    <row r="84" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A84" s="12" t="s">
+      <c r="J84" s="11"/>
+    </row>
+    <row r="85" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+      <c r="A85" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>713</v>
       </c>
-      <c r="C84" s="13" t="s">
+      <c r="C85" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="D84" s="13" t="s">
+      <c r="D85" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="E84" s="13">
+      <c r="E85" s="13">
         <v>1841</v>
       </c>
-      <c r="F84" s="13">
+      <c r="F85" s="13">
         <v>1921</v>
       </c>
-      <c r="G84" s="13" t="s">
+      <c r="G85" s="13" t="s">
         <v>885</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H85" t="s">
         <v>367</v>
       </c>
-      <c r="I84" s="13" t="s">
+      <c r="I85" s="13" t="s">
         <v>503</v>
       </c>
-      <c r="J84" s="11"/>
-    </row>
-    <row r="85" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A85" s="14" t="s">
+      <c r="J85" s="11"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>714</v>
       </c>
-      <c r="C85" s="15"/>
-      <c r="D85" s="15" t="s">
+      <c r="C86" s="15"/>
+      <c r="D86" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E85" s="15">
+      <c r="E86" s="15">
         <v>1821</v>
       </c>
-      <c r="F85" s="15">
+      <c r="F86" s="15">
         <v>1879</v>
       </c>
-      <c r="G85" s="15" t="s">
+      <c r="G86" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="H85" t="s">
+      <c r="H86" t="s">
         <v>369</v>
       </c>
-      <c r="I85" s="15" t="s">
+      <c r="I86" s="15" t="s">
         <v>533</v>
       </c>
-      <c r="J85" s="16"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A86" s="9" t="s">
+      <c r="J86" s="16"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>715</v>
       </c>
-      <c r="C86" s="10" t="s">
+      <c r="C87" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="D86" s="10" t="s">
+      <c r="D87" s="10" t="s">
         <v>370</v>
       </c>
-      <c r="E86" s="10">
+      <c r="E87" s="10">
         <v>1851</v>
       </c>
-      <c r="F86" s="10">
+      <c r="F87" s="10">
         <v>1921</v>
       </c>
-      <c r="G86" s="10" t="s">
+      <c r="G87" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="H86" t="s">
+      <c r="H87" t="s">
         <v>371</v>
       </c>
-      <c r="I86" s="10" t="s">
+      <c r="I87" s="10" t="s">
         <v>534</v>
       </c>
-      <c r="J86" s="18" t="s">
+      <c r="J87" s="18" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A87" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>716</v>
-      </c>
-      <c r="C87" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D87" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E87" s="13">
-        <v>1850</v>
-      </c>
-      <c r="F87" s="13">
-        <v>1918</v>
-      </c>
-      <c r="G87" s="13" t="s">
-        <v>887</v>
-      </c>
-      <c r="H87" t="s">
-        <v>372</v>
-      </c>
-      <c r="I87" s="13" t="s">
-        <v>502</v>
-      </c>
-      <c r="J87" s="11"/>
-    </row>
-    <row r="88" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A88" s="12" t="s">
         <v>154</v>
       </c>
       <c r="B88" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="C88" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D88" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E88" s="13">
+        <v>1850</v>
+      </c>
+      <c r="F88" s="13">
+        <v>1918</v>
+      </c>
+      <c r="G88" s="13" t="s">
+        <v>887</v>
+      </c>
+      <c r="H88" t="s">
+        <v>372</v>
+      </c>
+      <c r="I88" s="13" t="s">
+        <v>502</v>
+      </c>
+      <c r="J88" s="11"/>
+    </row>
+    <row r="89" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A89" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>717</v>
       </c>
-      <c r="C88" s="13" t="s">
+      <c r="C89" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="D88" s="13" t="s">
+      <c r="D89" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="E88" s="13">
+      <c r="E89" s="13">
         <v>1872</v>
       </c>
-      <c r="F88" s="13">
+      <c r="F89" s="13">
         <v>1962</v>
       </c>
-      <c r="G88" s="13" t="s">
+      <c r="G89" s="13" t="s">
         <v>886</v>
       </c>
-      <c r="H88" t="s">
+      <c r="H89" t="s">
         <v>373</v>
       </c>
-      <c r="I88" s="13" t="s">
+      <c r="I89" s="13" t="s">
         <v>501</v>
       </c>
-      <c r="J88" s="11"/>
-    </row>
-    <row r="89" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A89" s="12" t="s">
+      <c r="J89" s="11"/>
+    </row>
+    <row r="90" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A90" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>718</v>
       </c>
-      <c r="C89" s="13" t="s">
+      <c r="C90" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D89" s="13" t="s">
+      <c r="D90" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="E89" s="13">
+      <c r="E90" s="13">
         <v>1861</v>
       </c>
-      <c r="F89" s="13">
+      <c r="F90" s="13">
         <v>1939</v>
       </c>
-      <c r="G89" s="13" t="s">
+      <c r="G90" s="13" t="s">
         <v>888</v>
       </c>
-      <c r="H89" t="s">
+      <c r="H90" t="s">
         <v>374</v>
       </c>
-      <c r="I89" s="13" t="s">
+      <c r="I90" s="13" t="s">
         <v>500</v>
       </c>
-      <c r="J89" s="11"/>
-    </row>
-    <row r="90" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A90" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>719</v>
-      </c>
-      <c r="C90" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="D90" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="E90" s="13">
-        <v>1846</v>
-      </c>
-      <c r="F90" s="13">
-        <v>1920</v>
-      </c>
-      <c r="G90" s="13" t="s">
-        <v>889</v>
-      </c>
-      <c r="H90" t="s">
-        <v>375</v>
-      </c>
-      <c r="I90" s="13" t="s">
-        <v>499</v>
-      </c>
       <c r="J90" s="11"/>
     </row>
-    <row r="91" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" ht="75" x14ac:dyDescent="0.2">
       <c r="A91" s="12" t="s">
         <v>159</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C91" s="13" t="s">
         <v>160</v>
       </c>
       <c r="D91" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E91" s="13">
+        <v>1846</v>
+      </c>
+      <c r="F91" s="13">
+        <v>1920</v>
+      </c>
+      <c r="G91" s="13" t="s">
+        <v>889</v>
+      </c>
+      <c r="H91" t="s">
+        <v>375</v>
+      </c>
+      <c r="I91" s="13" t="s">
+        <v>499</v>
+      </c>
+      <c r="J91" s="11"/>
+    </row>
+    <row r="92" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A92" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D92" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="E91" s="13">
+      <c r="E92" s="13">
         <v>1872</v>
       </c>
-      <c r="F91" s="13">
+      <c r="F92" s="13">
         <v>1951</v>
       </c>
-      <c r="G91" s="13" t="s">
+      <c r="G92" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="H91" t="s">
+      <c r="H92" t="s">
         <v>376</v>
       </c>
-      <c r="I91" s="13" t="s">
+      <c r="I92" s="13" t="s">
         <v>498</v>
       </c>
-      <c r="J91" s="11"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A92" s="12" t="s">
+      <c r="J92" s="11"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A93" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>721</v>
       </c>
-      <c r="C92" s="13" t="s">
+      <c r="C93" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D92" s="13" t="s">
+      <c r="D93" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="E92" s="13">
+      <c r="E93" s="13">
         <v>1829</v>
       </c>
-      <c r="F92" s="13">
+      <c r="F93" s="13">
         <v>1910</v>
       </c>
-      <c r="G92" s="13" t="s">
+      <c r="G93" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="H92" t="s">
+      <c r="H93" t="s">
         <v>377</v>
       </c>
-      <c r="I92" s="13" t="s">
+      <c r="I93" s="13" t="s">
         <v>497</v>
       </c>
-      <c r="J92" s="11"/>
-    </row>
-    <row r="93" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A93" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>722</v>
-      </c>
-      <c r="C93" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E93" s="13">
-        <v>1835</v>
-      </c>
-      <c r="F93" s="13">
-        <v>1908</v>
-      </c>
-      <c r="G93" s="13" t="s">
-        <v>890</v>
-      </c>
-      <c r="H93" t="s">
-        <v>378</v>
-      </c>
-      <c r="I93" s="13" t="s">
-        <v>496</v>
-      </c>
-      <c r="J93" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J93" s="11"/>
+    </row>
+    <row r="94" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A94" s="12" t="s">
         <v>166</v>
       </c>
       <c r="B94" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D94" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="E94" s="13">
+        <v>1835</v>
+      </c>
+      <c r="F94" s="13">
+        <v>1908</v>
+      </c>
+      <c r="G94" s="13" t="s">
+        <v>890</v>
+      </c>
+      <c r="H94" t="s">
+        <v>378</v>
+      </c>
+      <c r="I94" s="13" t="s">
+        <v>496</v>
+      </c>
+      <c r="J94" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="A95" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>723</v>
       </c>
-      <c r="C94" s="13" t="s">
+      <c r="C95" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="D94" s="13" t="s">
+      <c r="D95" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E94" s="13">
+      <c r="E95" s="13">
         <v>1850</v>
       </c>
-      <c r="F94" s="13">
+      <c r="F95" s="13">
         <v>1926</v>
       </c>
-      <c r="G94" s="13" t="s">
+      <c r="G95" s="13" t="s">
         <v>891</v>
       </c>
-      <c r="H94" t="s">
+      <c r="H95" t="s">
         <v>379</v>
       </c>
-      <c r="I94" s="13" t="s">
+      <c r="I95" s="13" t="s">
         <v>495</v>
       </c>
-      <c r="J94" s="11"/>
-    </row>
-    <row r="95" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A95" s="12" t="s">
+      <c r="J95" s="11"/>
+    </row>
+    <row r="96" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A96" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>724</v>
       </c>
-      <c r="C95" s="13" t="s">
+      <c r="C96" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D95" s="13" t="s">
+      <c r="D96" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="E95" s="13">
+      <c r="E96" s="13">
         <v>1860</v>
       </c>
-      <c r="F95" s="13">
+      <c r="F96" s="13">
         <v>1945</v>
       </c>
-      <c r="G95" s="13" t="s">
+      <c r="G96" s="13" t="s">
         <v>892</v>
       </c>
-      <c r="H95" t="s">
+      <c r="H96" t="s">
         <v>380</v>
       </c>
-      <c r="I95" s="13" t="s">
+      <c r="I96" s="13" t="s">
         <v>494</v>
       </c>
-      <c r="J95" s="11"/>
-    </row>
-    <row r="96" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A96" s="12" t="s">
+      <c r="J96" s="11"/>
+    </row>
+    <row r="97" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A97" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="C96" s="13" t="s">
+      <c r="C97" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="D96" s="13" t="s">
+      <c r="D97" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="E96" s="13">
+      <c r="E97" s="13">
         <v>1845</v>
       </c>
-      <c r="F96" s="13">
+      <c r="F97" s="13">
         <v>1929</v>
       </c>
-      <c r="G96" s="13" t="s">
+      <c r="G97" s="13" t="s">
         <v>893</v>
       </c>
-      <c r="H96" t="s">
+      <c r="H97" t="s">
         <v>381</v>
       </c>
-      <c r="I96" s="13" t="s">
+      <c r="I97" s="13" t="s">
         <v>493</v>
       </c>
-      <c r="J96" s="11"/>
-    </row>
-    <row r="97" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A97" s="14" t="s">
+      <c r="J97" s="11"/>
+    </row>
+    <row r="98" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A98" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>726</v>
       </c>
-      <c r="C97" s="15" t="s">
+      <c r="C98" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D97" s="15" t="s">
+      <c r="D98" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="E97" s="15">
+      <c r="E98" s="15">
         <v>1844</v>
       </c>
-      <c r="F97" s="15">
+      <c r="F98" s="15">
         <v>1910</v>
       </c>
-      <c r="G97" s="15" t="s">
+      <c r="G98" s="15" t="s">
         <v>894</v>
       </c>
-      <c r="H97" t="s">
+      <c r="H98" t="s">
         <v>382</v>
       </c>
-      <c r="I97" s="15" t="s">
+      <c r="I98" s="15" t="s">
         <v>492</v>
       </c>
-      <c r="J97" s="16"/>
-    </row>
-    <row r="98" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A98" s="12" t="s">
+      <c r="J98" s="16"/>
+    </row>
+    <row r="99" spans="1:10" ht="105" x14ac:dyDescent="0.2">
+      <c r="A99" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B99" s="2" t="s">
         <v>727</v>
       </c>
-      <c r="C98" s="13" t="s">
+      <c r="C99" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D98" s="13" t="s">
+      <c r="D99" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="E98" s="13">
+      <c r="E99" s="13">
         <v>1846</v>
       </c>
-      <c r="F98" s="13">
+      <c r="F99" s="13">
         <v>1916</v>
       </c>
-      <c r="G98" s="13" t="s">
+      <c r="G99" s="13" t="s">
         <v>895</v>
       </c>
-      <c r="H98" t="s">
+      <c r="H99" t="s">
         <v>383</v>
       </c>
-      <c r="I98" s="13" t="s">
+      <c r="I99" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="J98" s="11"/>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A99" s="12" t="s">
+      <c r="J99" s="11"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A100" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="C99" s="13"/>
-      <c r="D99" s="13" t="s">
+      <c r="C100" s="13"/>
+      <c r="D100" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="E99" s="13">
+      <c r="E100" s="13">
         <v>1838</v>
       </c>
-      <c r="F99" s="13">
+      <c r="F100" s="13">
         <v>1925</v>
       </c>
-      <c r="G99" s="13" t="s">
+      <c r="G100" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="H99" t="s">
+      <c r="H100" t="s">
         <v>384</v>
       </c>
-      <c r="I99" s="13" t="s">
+      <c r="I100" s="13" t="s">
         <v>535</v>
       </c>
-      <c r="J99" s="11"/>
-    </row>
-    <row r="100" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A100" s="14" t="s">
+      <c r="J100" s="11"/>
+    </row>
+    <row r="101" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A101" s="14" t="s">
         <v>823</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>824</v>
       </c>
-      <c r="C100" s="15" t="s">
+      <c r="C101" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="D100" s="15" t="s">
+      <c r="D101" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="E100" s="15"/>
-      <c r="F100" s="15">
+      <c r="E101" s="15"/>
+      <c r="F101" s="15">
         <v>1916</v>
       </c>
-      <c r="G100" s="15"/>
-      <c r="H100" s="15"/>
-      <c r="I100" s="15" t="s">
+      <c r="G101" s="15"/>
+      <c r="H101" s="15"/>
+      <c r="I101" s="15" t="s">
         <v>490</v>
       </c>
-      <c r="J100" s="16"/>
-    </row>
-    <row r="101" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A101" s="14" t="s">
+      <c r="J101" s="16"/>
+    </row>
+    <row r="102" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A102" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>729</v>
       </c>
-      <c r="C101" s="15" t="s">
+      <c r="C102" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D101" s="15" t="s">
+      <c r="D102" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="E101" s="15">
+      <c r="E102" s="15">
         <v>1863</v>
       </c>
-      <c r="F101" s="15">
+      <c r="F102" s="15">
         <v>1931</v>
       </c>
-      <c r="G101" s="15" t="s">
+      <c r="G102" s="15" t="s">
         <v>896</v>
       </c>
-      <c r="H101" t="s">
+      <c r="H102" t="s">
         <v>385</v>
       </c>
-      <c r="I101" s="15" t="s">
+      <c r="I102" s="15" t="s">
         <v>489</v>
       </c>
-      <c r="J101" s="16"/>
-    </row>
-    <row r="102" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A102" s="12" t="s">
+      <c r="J102" s="16"/>
+    </row>
+    <row r="103" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="A103" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>730</v>
       </c>
-      <c r="C102" s="13" t="s">
+      <c r="C103" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D102" s="13" t="s">
+      <c r="D103" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="E102" s="13">
+      <c r="E103" s="13">
         <v>1846</v>
       </c>
-      <c r="F102" s="13">
+      <c r="F103" s="13">
         <v>1914</v>
       </c>
-      <c r="G102" s="13" t="s">
+      <c r="G103" s="13" t="s">
         <v>897</v>
       </c>
-      <c r="H102" t="s">
+      <c r="H103" t="s">
         <v>386</v>
       </c>
-      <c r="I102" s="13" t="s">
+      <c r="I103" s="13" t="s">
         <v>536</v>
       </c>
-      <c r="J102" s="11"/>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A103" s="19" t="s">
+      <c r="J103" s="11"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A104" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B104" s="2" t="s">
         <v>825</v>
       </c>
-      <c r="C103" s="39"/>
-      <c r="D103" s="39"/>
-      <c r="E103" s="39"/>
-      <c r="F103" s="39"/>
-      <c r="G103" s="39"/>
-      <c r="H103" s="39"/>
-      <c r="I103" s="20" t="s">
+      <c r="C104" s="39"/>
+      <c r="D104" s="39"/>
+      <c r="E104" s="39"/>
+      <c r="F104" s="39"/>
+      <c r="G104" s="39"/>
+      <c r="H104" s="39"/>
+      <c r="I104" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="J103" s="40"/>
-    </row>
-    <row r="104" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A104" s="19" t="s">
+      <c r="J104" s="40"/>
+    </row>
+    <row r="105" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A105" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>731</v>
       </c>
-      <c r="C104" s="20" t="s">
+      <c r="C105" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="D104" s="20" t="s">
+      <c r="D105" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="E104" s="20">
+      <c r="E105" s="20">
         <v>1855</v>
       </c>
-      <c r="F104" s="20">
+      <c r="F105" s="20">
         <v>1928</v>
       </c>
-      <c r="G104" s="20" t="s">
+      <c r="G105" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="H104" t="s">
+      <c r="H105" t="s">
         <v>387</v>
       </c>
-      <c r="I104" s="20" t="s">
+      <c r="I105" s="20" t="s">
         <v>537</v>
       </c>
-      <c r="J104" s="21" t="s">
+      <c r="J105" s="21" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A105" s="12" t="s">
+    <row r="106" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A106" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B106" s="2" t="s">
         <v>732</v>
       </c>
-      <c r="C105" s="13" t="s">
+      <c r="C106" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D105" s="13" t="s">
+      <c r="D106" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="E105" s="13">
+      <c r="E106" s="13">
         <v>1853</v>
       </c>
-      <c r="F105" s="13">
+      <c r="F106" s="13">
         <v>1910</v>
       </c>
-      <c r="G105" s="13" t="s">
+      <c r="G106" s="13" t="s">
         <v>898</v>
       </c>
-      <c r="H105" t="s">
+      <c r="H106" t="s">
         <v>389</v>
       </c>
-      <c r="I105" s="13" t="s">
+      <c r="I106" s="13" t="s">
         <v>488</v>
       </c>
-      <c r="J105" s="11"/>
-    </row>
-    <row r="106" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A106" s="12" t="s">
+      <c r="J106" s="11"/>
+    </row>
+    <row r="107" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A107" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B107" s="2" t="s">
         <v>733</v>
-      </c>
-      <c r="C106" s="13"/>
-      <c r="D106" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="E106" s="13">
-        <v>1850</v>
-      </c>
-      <c r="F106" s="13">
-        <v>1918</v>
-      </c>
-      <c r="G106" s="13" t="s">
-        <v>899</v>
-      </c>
-      <c r="H106" t="s">
-        <v>390</v>
-      </c>
-      <c r="I106" s="13" t="s">
-        <v>487</v>
-      </c>
-      <c r="J106" s="11"/>
-    </row>
-    <row r="107" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A107" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>734</v>
       </c>
       <c r="C107" s="13"/>
       <c r="D107" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E107" s="13">
+        <v>1850</v>
+      </c>
+      <c r="F107" s="13">
+        <v>1918</v>
+      </c>
+      <c r="G107" s="13" t="s">
+        <v>899</v>
+      </c>
+      <c r="H107" t="s">
+        <v>390</v>
+      </c>
+      <c r="I107" s="13" t="s">
+        <v>487</v>
+      </c>
+      <c r="J107" s="11"/>
+    </row>
+    <row r="108" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A108" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="C108" s="13"/>
+      <c r="D108" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="E107" s="13">
+      <c r="E108" s="13">
         <v>1856</v>
       </c>
-      <c r="F107" s="13">
+      <c r="F108" s="13">
         <v>1908</v>
       </c>
-      <c r="G107" s="13" t="s">
+      <c r="G108" s="13" t="s">
         <v>900</v>
       </c>
-      <c r="H107" t="s">
+      <c r="H108" t="s">
         <v>391</v>
       </c>
-      <c r="I107" s="13" t="s">
+      <c r="I108" s="13" t="s">
         <v>486</v>
       </c>
-      <c r="J107" s="11"/>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A108" s="12" t="s">
+      <c r="J108" s="11"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A109" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B109" s="2" t="s">
         <v>735</v>
       </c>
-      <c r="C108" s="13" t="s">
+      <c r="C109" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="D108" s="13" t="s">
+      <c r="D109" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="E108" s="13">
+      <c r="E109" s="13">
         <v>1847</v>
       </c>
-      <c r="F108" s="13">
+      <c r="F109" s="13">
         <v>1907</v>
       </c>
-      <c r="G108" s="13"/>
-      <c r="H108" s="13"/>
-      <c r="I108" s="13" t="s">
-        <v>485</v>
-      </c>
-      <c r="J108" s="11"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A109" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>826</v>
-      </c>
-      <c r="C109" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="D109" s="13"/>
-      <c r="E109" s="13"/>
-      <c r="F109" s="13"/>
       <c r="G109" s="13"/>
       <c r="H109" s="13"/>
       <c r="I109" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="J109" s="11"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A110" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="J109" s="11"/>
-    </row>
-    <row r="110" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A110" s="12" t="s">
+      <c r="B110" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="C110" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13"/>
+      <c r="F110" s="13"/>
+      <c r="G110" s="13"/>
+      <c r="H110" s="13"/>
+      <c r="I110" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="J110" s="11"/>
+    </row>
+    <row r="111" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+      <c r="A111" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B111" s="2" t="s">
         <v>736</v>
       </c>
-      <c r="C110" s="13" t="s">
+      <c r="C111" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="D110" s="13" t="s">
+      <c r="D111" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="E110" s="13">
+      <c r="E111" s="13">
         <v>1858</v>
       </c>
-      <c r="F110" s="13">
+      <c r="F111" s="13">
         <v>1917</v>
       </c>
-      <c r="G110" s="13" t="s">
+      <c r="G111" s="13" t="s">
         <v>901</v>
       </c>
-      <c r="H110" t="s">
+      <c r="H111" t="s">
         <v>392</v>
       </c>
-      <c r="I110" s="13" t="s">
+      <c r="I111" s="13" t="s">
         <v>484</v>
       </c>
-      <c r="J110" s="11" t="s">
+      <c r="J111" s="11" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A111" s="12" t="s">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A112" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>827</v>
       </c>
-      <c r="C111" s="13" t="s">
+      <c r="C112" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D111" s="13"/>
-      <c r="E111" s="13"/>
-      <c r="F111" s="13"/>
-      <c r="G111" s="13"/>
-      <c r="H111" s="13"/>
-      <c r="I111" s="13" t="s">
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="13"/>
+      <c r="G112" s="13"/>
+      <c r="H112" s="13"/>
+      <c r="I112" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="J111" s="11"/>
-    </row>
-    <row r="112" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="12" t="s">
+      <c r="J112" s="11"/>
+    </row>
+    <row r="113" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="A113" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="C112" s="13"/>
-      <c r="D112" s="13" t="s">
+      <c r="C113" s="13"/>
+      <c r="D113" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E112" s="13">
+      <c r="E113" s="13">
         <v>1853</v>
       </c>
-      <c r="F112" s="13">
+      <c r="F113" s="13">
         <v>1927</v>
       </c>
-      <c r="G112" s="13" t="s">
+      <c r="G113" s="13" t="s">
         <v>902</v>
       </c>
-      <c r="H112" t="s">
+      <c r="H113" t="s">
         <v>393</v>
       </c>
-      <c r="I112" s="13" t="s">
+      <c r="I113" s="13" t="s">
         <v>483</v>
       </c>
-      <c r="J112" s="11"/>
-    </row>
-    <row r="113" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A113" s="14" t="s">
+      <c r="J113" s="11"/>
+    </row>
+    <row r="114" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+      <c r="A114" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>738</v>
       </c>
-      <c r="C113" s="15"/>
-      <c r="D113" s="15" t="s">
+      <c r="C114" s="15"/>
+      <c r="D114" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="E113" s="15">
+      <c r="E114" s="15">
         <v>1868</v>
       </c>
-      <c r="F113" s="15">
+      <c r="F114" s="15">
         <v>1932</v>
       </c>
-      <c r="G113" s="15" t="s">
+      <c r="G114" s="15" t="s">
         <v>903</v>
       </c>
-      <c r="H113" t="s">
+      <c r="H114" t="s">
         <v>394</v>
       </c>
-      <c r="I113" s="15" t="s">
+      <c r="I114" s="15" t="s">
         <v>538</v>
       </c>
-      <c r="J113" s="16"/>
-    </row>
-    <row r="114" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A114" s="12" t="s">
+      <c r="J114" s="16"/>
+    </row>
+    <row r="115" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+      <c r="A115" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B115" s="2" t="s">
         <v>739</v>
       </c>
-      <c r="C114" s="13" t="s">
+      <c r="C115" s="13" t="s">
         <v>904</v>
       </c>
-      <c r="D114" s="13" t="s">
+      <c r="D115" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="E114" s="13">
+      <c r="E115" s="13">
         <v>1834</v>
       </c>
-      <c r="F114" s="13">
+      <c r="F115" s="13">
         <v>1914</v>
       </c>
-      <c r="G114" s="13" t="s">
+      <c r="G115" s="13" t="s">
         <v>905</v>
       </c>
-      <c r="H114" t="s">
+      <c r="H115" t="s">
         <v>395</v>
       </c>
-      <c r="I114" s="13" t="s">
+      <c r="I115" s="13" t="s">
         <v>539</v>
       </c>
-      <c r="J114" s="18"/>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A115" s="12" t="s">
+      <c r="J115" s="18"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A116" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B116" s="2" t="s">
         <v>740</v>
       </c>
-      <c r="C115" s="13" t="s">
+      <c r="C116" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="D115" s="13" t="s">
+      <c r="D116" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="E115" s="13">
+      <c r="E116" s="13">
         <v>1797</v>
       </c>
-      <c r="F115" s="13">
+      <c r="F116" s="13">
         <v>1875</v>
       </c>
-      <c r="G115" s="13" t="s">
+      <c r="G116" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="H115" t="s">
+      <c r="H116" t="s">
         <v>396</v>
       </c>
-      <c r="I115" s="13" t="s">
+      <c r="I116" s="13" t="s">
         <v>540</v>
       </c>
-      <c r="J115" s="18"/>
-    </row>
-    <row r="116" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A116" s="12" t="s">
+      <c r="J116" s="18"/>
+    </row>
+    <row r="117" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A117" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B117" s="2" t="s">
         <v>741</v>
       </c>
-      <c r="C116" s="13" t="s">
+      <c r="C117" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="D116" s="13" t="s">
+      <c r="D117" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E116" s="13">
+      <c r="E117" s="13">
         <v>1857</v>
       </c>
-      <c r="F116" s="13">
+      <c r="F117" s="13">
         <v>1912</v>
       </c>
-      <c r="G116" s="13" t="s">
+      <c r="G117" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="H116" t="s">
+      <c r="H117" t="s">
         <v>397</v>
       </c>
-      <c r="I116" s="13" t="s">
+      <c r="I117" s="13" t="s">
         <v>541</v>
       </c>
-      <c r="J116" s="11" t="s">
+      <c r="J117" s="11" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A117" s="12" t="s">
+    <row r="118" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A118" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>742</v>
       </c>
-      <c r="C117" s="13" t="s">
+      <c r="C118" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="D117" s="13" t="s">
+      <c r="D118" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="E117" s="13">
+      <c r="E118" s="13">
         <v>1853</v>
       </c>
-      <c r="F117" s="13">
+      <c r="F118" s="13">
         <v>1914</v>
       </c>
-      <c r="G117" s="13" t="s">
+      <c r="G118" s="13" t="s">
         <v>906</v>
       </c>
-      <c r="H117" t="s">
+      <c r="H118" t="s">
         <v>398</v>
       </c>
-      <c r="I117" s="10" t="s">
+      <c r="I118" s="10" t="s">
         <v>482</v>
       </c>
-      <c r="J117" s="18"/>
-    </row>
-    <row r="118" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A118" s="22" t="s">
+      <c r="J118" s="18"/>
+    </row>
+    <row r="119" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A119" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B119" s="2" t="s">
         <v>743</v>
       </c>
-      <c r="C118" s="15" t="s">
+      <c r="C119" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="D118" s="23" t="s">
+      <c r="D119" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="E118" s="23">
+      <c r="E119" s="23">
         <v>1845</v>
       </c>
-      <c r="F118" s="23">
+      <c r="F119" s="23">
         <v>1933</v>
       </c>
-      <c r="G118" s="15" t="s">
+      <c r="G119" s="15" t="s">
         <v>907</v>
       </c>
-      <c r="H118" t="s">
+      <c r="H119" t="s">
         <v>399</v>
       </c>
-      <c r="I118" s="15" t="s">
+      <c r="I119" s="15" t="s">
         <v>481</v>
       </c>
-      <c r="J118" s="24"/>
-    </row>
-    <row r="119" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A119" s="12" t="s">
+      <c r="J119" s="24"/>
+    </row>
+    <row r="120" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="A120" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B120" s="2" t="s">
         <v>744</v>
       </c>
-      <c r="C119" s="13" t="s">
+      <c r="C120" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D119" s="13" t="s">
+      <c r="D120" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E119" s="13">
+      <c r="E120" s="13">
         <v>1831</v>
       </c>
-      <c r="F119" s="13">
+      <c r="F120" s="13">
         <v>1903</v>
       </c>
-      <c r="G119" s="13" t="s">
+      <c r="G120" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="H119" t="s">
+      <c r="H120" t="s">
         <v>400</v>
       </c>
-      <c r="I119" s="13" t="s">
+      <c r="I120" s="13" t="s">
         <v>542</v>
       </c>
-      <c r="J119" s="11"/>
-    </row>
-    <row r="120" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A120" s="12" t="s">
+      <c r="J120" s="11"/>
+    </row>
+    <row r="121" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A121" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B121" s="2" t="s">
         <v>745</v>
       </c>
-      <c r="C120" s="13" t="s">
+      <c r="C121" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D120" s="13" t="s">
+      <c r="D121" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="E120" s="13">
+      <c r="E121" s="13">
         <v>1869</v>
       </c>
-      <c r="F120" s="13">
+      <c r="F121" s="13">
         <v>1951</v>
       </c>
-      <c r="G120" s="13" t="s">
+      <c r="G121" s="13" t="s">
         <v>915</v>
       </c>
-      <c r="H120" s="13"/>
-      <c r="I120" s="13" t="s">
+      <c r="H121" s="13"/>
+      <c r="I121" s="13" t="s">
         <v>480</v>
       </c>
-      <c r="J120" s="11"/>
-    </row>
-    <row r="121" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A121" s="12" t="s">
+      <c r="J121" s="11"/>
+    </row>
+    <row r="122" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A122" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B122" s="2" t="s">
         <v>746</v>
       </c>
-      <c r="C121" s="13" t="s">
+      <c r="C122" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="D121" s="13" t="s">
+      <c r="D122" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="E121" s="13">
+      <c r="E122" s="13">
         <v>1838</v>
       </c>
-      <c r="F121" s="13">
+      <c r="F122" s="13">
         <v>1917</v>
       </c>
-      <c r="G121" s="13" t="s">
+      <c r="G122" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="H121" t="s">
+      <c r="H122" t="s">
         <v>401</v>
       </c>
-      <c r="I121" s="13" t="s">
+      <c r="I122" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="J121" s="11"/>
-    </row>
-    <row r="122" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A122" s="12" t="s">
+      <c r="J122" s="11"/>
+    </row>
+    <row r="123" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="A123" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B123" s="2" t="s">
         <v>747</v>
       </c>
-      <c r="C122" s="13" t="s">
+      <c r="C123" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D122" s="13" t="s">
+      <c r="D123" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="E122" s="13">
+      <c r="E123" s="13">
         <v>1841</v>
       </c>
-      <c r="F122" s="13">
+      <c r="F123" s="13">
         <v>1907</v>
       </c>
-      <c r="G122" s="13" t="s">
+      <c r="G123" s="13" t="s">
         <v>908</v>
       </c>
-      <c r="H122" t="s">
+      <c r="H123" t="s">
         <v>402</v>
       </c>
-      <c r="I122" s="13" t="s">
+      <c r="I123" s="13" t="s">
         <v>543</v>
       </c>
-      <c r="J122" s="11"/>
-    </row>
-    <row r="123" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A123" s="12" t="s">
+      <c r="J123" s="11"/>
+    </row>
+    <row r="124" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+      <c r="A124" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B124" s="2" t="s">
         <v>748</v>
       </c>
-      <c r="C123" s="13" t="s">
+      <c r="C124" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D123" s="13" t="s">
+      <c r="D124" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="E123" s="13">
+      <c r="E124" s="13">
         <v>1842</v>
       </c>
-      <c r="F123" s="13">
+      <c r="F124" s="13">
         <v>1921</v>
       </c>
-      <c r="G123" s="13" t="s">
+      <c r="G124" s="13" t="s">
         <v>909</v>
       </c>
-      <c r="H123" t="s">
+      <c r="H124" t="s">
         <v>403</v>
       </c>
-      <c r="I123" s="13" t="s">
+      <c r="I124" s="13" t="s">
         <v>544</v>
       </c>
-      <c r="J123" s="11"/>
-    </row>
-    <row r="124" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A124" s="12" t="s">
+      <c r="J124" s="11"/>
+    </row>
+    <row r="125" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+      <c r="A125" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="B125" s="2" t="s">
         <v>749</v>
       </c>
-      <c r="C124" s="13" t="s">
+      <c r="C125" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="D124" s="13" t="s">
+      <c r="D125" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="E124" s="13">
+      <c r="E125" s="13">
         <v>1858</v>
       </c>
-      <c r="F124" s="13">
+      <c r="F125" s="13">
         <v>1926</v>
       </c>
-      <c r="G124" s="13" t="s">
+      <c r="G125" s="13" t="s">
         <v>910</v>
       </c>
-      <c r="H124" t="s">
+      <c r="H125" t="s">
         <v>404</v>
       </c>
-      <c r="I124" s="13" t="s">
+      <c r="I125" s="13" t="s">
         <v>478</v>
       </c>
-      <c r="J124" s="11"/>
-    </row>
-    <row r="125" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A125" s="12" t="s">
+      <c r="J125" s="11"/>
+    </row>
+    <row r="126" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A126" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="B126" s="2" t="s">
         <v>750</v>
       </c>
-      <c r="C125" s="13" t="s">
+      <c r="C126" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="D125" s="13" t="s">
+      <c r="D126" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E125" s="13">
+      <c r="E126" s="13">
         <v>1859</v>
       </c>
-      <c r="F125" s="13">
+      <c r="F126" s="13">
         <v>1913</v>
       </c>
-      <c r="G125" s="13" t="s">
+      <c r="G126" s="13" t="s">
         <v>911</v>
       </c>
-      <c r="H125" t="s">
+      <c r="H126" t="s">
         <v>405</v>
       </c>
-      <c r="I125" s="13" t="s">
+      <c r="I126" s="13" t="s">
         <v>477</v>
       </c>
-      <c r="J125" s="11"/>
-    </row>
-    <row r="126" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A126" s="12" t="s">
+      <c r="J126" s="11"/>
+    </row>
+    <row r="127" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A127" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="B127" s="2" t="s">
         <v>751</v>
       </c>
-      <c r="C126" s="13" t="s">
+      <c r="C127" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D126" s="13" t="s">
+      <c r="D127" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="E126" s="13">
+      <c r="E127" s="13">
         <v>1836</v>
       </c>
-      <c r="F126" s="13">
+      <c r="F127" s="13">
         <v>1914</v>
       </c>
-      <c r="G126" s="13" t="s">
+      <c r="G127" s="13" t="s">
         <v>912</v>
       </c>
-      <c r="H126" t="s">
+      <c r="H127" t="s">
         <v>406</v>
       </c>
-      <c r="I126" s="13" t="s">
+      <c r="I127" s="13" t="s">
         <v>476</v>
       </c>
-      <c r="J126" s="11"/>
-    </row>
-    <row r="127" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A127" s="12" t="s">
+      <c r="J127" s="11"/>
+    </row>
+    <row r="128" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="A128" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B128" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="C127" s="13" t="s">
+      <c r="C128" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D127" s="13" t="s">
+      <c r="D128" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="E127" s="13">
+      <c r="E128" s="13">
         <v>1866</v>
       </c>
-      <c r="F127" s="13">
+      <c r="F128" s="13">
         <v>1934</v>
       </c>
-      <c r="G127" s="13" t="s">
+      <c r="G128" s="13" t="s">
         <v>913</v>
       </c>
-      <c r="H127" t="s">
+      <c r="H128" t="s">
         <v>407</v>
       </c>
-      <c r="I127" s="13" t="s">
+      <c r="I128" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="J127" s="11"/>
-    </row>
-    <row r="128" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A128" s="12" t="s">
+      <c r="J128" s="11"/>
+    </row>
+    <row r="129" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="A129" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B129" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="C128" s="13" t="s">
+      <c r="C129" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D128" s="13" t="s">
+      <c r="D129" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E128" s="13">
+      <c r="E129" s="13">
         <v>1860</v>
       </c>
-      <c r="F128" s="13">
+      <c r="F129" s="13">
         <v>1936</v>
       </c>
-      <c r="G128" s="13" t="s">
+      <c r="G129" s="13" t="s">
         <v>914</v>
       </c>
-      <c r="H128" t="s">
+      <c r="H129" t="s">
         <v>408</v>
       </c>
-      <c r="I128" s="13" t="s">
+      <c r="I129" s="13" t="s">
         <v>474</v>
       </c>
-      <c r="J128" s="11" t="s">
+      <c r="J129" s="11" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A129" s="12" t="s">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A130" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="B130" s="2" t="s">
         <v>754</v>
       </c>
-      <c r="C129" s="13"/>
-      <c r="D129" s="13" t="s">
+      <c r="C130" s="13"/>
+      <c r="D130" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="E129" s="13">
+      <c r="E130" s="13">
         <v>1847</v>
-      </c>
-      <c r="F129" s="13">
-        <v>1917</v>
-      </c>
-      <c r="G129" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="H129" t="s">
-        <v>409</v>
-      </c>
-      <c r="I129" s="13" t="s">
-        <v>473</v>
-      </c>
-      <c r="J129" s="11"/>
-    </row>
-    <row r="130" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A130" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>755</v>
-      </c>
-      <c r="C130" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D130" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="E130" s="13">
-        <v>1849</v>
       </c>
       <c r="F130" s="13">
         <v>1917</v>
       </c>
       <c r="G130" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="H130" t="s">
+        <v>409</v>
+      </c>
+      <c r="I130" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="J130" s="11"/>
+    </row>
+    <row r="131" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A131" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="C131" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D131" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="E131" s="13">
+        <v>1849</v>
+      </c>
+      <c r="F131" s="13">
+        <v>1917</v>
+      </c>
+      <c r="G131" s="13" t="s">
         <v>916</v>
       </c>
-      <c r="H130" t="s">
+      <c r="H131" t="s">
         <v>410</v>
       </c>
-      <c r="I130" s="13" t="s">
+      <c r="I131" s="13" t="s">
         <v>472</v>
       </c>
-      <c r="J130" s="11"/>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A131" s="12" t="s">
+      <c r="J131" s="11"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A132" s="12" t="s">
         <v>412</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B132" s="2" t="s">
         <v>756</v>
       </c>
-      <c r="C131" s="13"/>
-      <c r="D131" s="13" t="s">
+      <c r="C132" s="13"/>
+      <c r="D132" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="E131" s="13">
+      <c r="E132" s="13">
         <v>1823</v>
       </c>
-      <c r="F131" s="13">
+      <c r="F132" s="13">
         <v>1896</v>
       </c>
-      <c r="G131" s="13" t="s">
+      <c r="G132" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="H131" t="s">
+      <c r="H132" t="s">
         <v>411</v>
       </c>
-      <c r="I131" s="13" t="s">
+      <c r="I132" s="13" t="s">
         <v>545</v>
       </c>
-      <c r="J131" s="11" t="s">
+      <c r="J132" s="11" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A132" s="9" t="s">
+    <row r="133" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A133" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="B133" s="2" t="s">
         <v>757</v>
       </c>
-      <c r="C132" s="10"/>
-      <c r="D132" s="10" t="s">
+      <c r="C133" s="10"/>
+      <c r="D133" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="E132" s="10">
+      <c r="E133" s="10">
         <v>1869</v>
       </c>
-      <c r="F132" s="10">
+      <c r="F133" s="10">
         <v>1943</v>
       </c>
-      <c r="G132" s="13" t="s">
+      <c r="G133" s="13" t="s">
         <v>917</v>
       </c>
-      <c r="H132" t="s">
+      <c r="H133" t="s">
         <v>414</v>
       </c>
-      <c r="I132" s="10" t="s">
+      <c r="I133" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="J132" s="18" t="s">
+      <c r="J133" s="18" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A133" s="12" t="s">
+    <row r="134" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="A134" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="B134" s="2" t="s">
         <v>758</v>
       </c>
-      <c r="C133" s="13" t="s">
+      <c r="C134" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D133" s="13" t="s">
+      <c r="D134" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="E133" s="13">
+      <c r="E134" s="13">
         <v>1846</v>
       </c>
-      <c r="F133" s="13">
+      <c r="F134" s="13">
         <v>1907</v>
       </c>
-      <c r="G133" s="13" t="s">
+      <c r="G134" s="13" t="s">
         <v>918</v>
       </c>
-      <c r="H133" t="s">
+      <c r="H134" t="s">
         <v>416</v>
       </c>
-      <c r="I133" s="13" t="s">
+      <c r="I134" s="13" t="s">
         <v>470</v>
       </c>
-      <c r="J133" s="11"/>
-    </row>
-    <row r="134" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A134" s="12" t="s">
+      <c r="J134" s="11"/>
+    </row>
+    <row r="135" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+      <c r="A135" s="12" t="s">
         <v>833</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="B135" s="2" t="s">
         <v>835</v>
       </c>
-      <c r="C134" s="13" t="s">
+      <c r="C135" s="13" t="s">
         <v>279</v>
       </c>
-      <c r="D134" s="13" t="s">
+      <c r="D135" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="E134" s="13">
+      <c r="E135" s="13">
         <v>1847</v>
       </c>
-      <c r="F134" s="13">
+      <c r="F135" s="13">
         <v>1921</v>
       </c>
-      <c r="G134" s="42" t="s">
+      <c r="G135" s="42" t="s">
         <v>919</v>
       </c>
-      <c r="H134" s="41" t="s">
+      <c r="H135" s="41" t="s">
         <v>834</v>
       </c>
-      <c r="I134" s="13" t="s">
+      <c r="I135" s="13" t="s">
         <v>836</v>
       </c>
-      <c r="J134" s="11"/>
-    </row>
-    <row r="135" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A135" s="9" t="s">
+      <c r="J135" s="11"/>
+    </row>
+    <row r="136" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A136" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B136" s="2" t="s">
         <v>759</v>
       </c>
-      <c r="C135" s="13"/>
-      <c r="D135" s="13" t="s">
+      <c r="C136" s="13"/>
+      <c r="D136" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="E135" s="13">
+      <c r="E136" s="13">
         <v>1815</v>
       </c>
-      <c r="F135" s="13">
+      <c r="F136" s="13">
         <v>1905</v>
       </c>
-      <c r="G135" s="13" t="s">
+      <c r="G136" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="H135" t="s">
+      <c r="H136" t="s">
         <v>417</v>
       </c>
-      <c r="I135" s="13" t="s">
+      <c r="I136" s="13" t="s">
         <v>469</v>
       </c>
-      <c r="J135" s="11" t="s">
+      <c r="J136" s="11" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A136" s="12" t="s">
+    <row r="137" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+      <c r="A137" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B137" s="2" t="s">
         <v>760</v>
       </c>
-      <c r="C136" s="13" t="s">
+      <c r="C137" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D136" s="13" t="s">
+      <c r="D137" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E136" s="13">
+      <c r="E137" s="13">
         <v>1859</v>
       </c>
-      <c r="F136" s="13" t="s">
+      <c r="F137" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="G136" s="13" t="s">
+      <c r="G137" s="13" t="s">
         <v>920</v>
       </c>
-      <c r="H136" t="s">
+      <c r="H137" t="s">
         <v>418</v>
       </c>
-      <c r="I136" s="13" t="s">
+      <c r="I137" s="13" t="s">
         <v>546</v>
       </c>
-      <c r="J136" s="11"/>
-    </row>
-    <row r="137" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A137" s="12" t="s">
+      <c r="J137" s="11"/>
+    </row>
+    <row r="138" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A138" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="B138" s="2" t="s">
         <v>761</v>
       </c>
-      <c r="C137" s="13"/>
-      <c r="D137" s="13" t="s">
+      <c r="C138" s="13"/>
+      <c r="D138" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="E137" s="13">
+      <c r="E138" s="13">
         <v>1843</v>
       </c>
-      <c r="F137" s="13">
+      <c r="F138" s="13">
         <v>1915</v>
       </c>
-      <c r="G137" s="13" t="s">
+      <c r="G138" s="13" t="s">
         <v>921</v>
       </c>
-      <c r="H137" t="s">
+      <c r="H138" t="s">
         <v>419</v>
       </c>
-      <c r="I137" s="13" t="s">
+      <c r="I138" s="13" t="s">
         <v>547</v>
       </c>
-      <c r="J137" s="11"/>
-    </row>
-    <row r="138" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A138" s="12" t="s">
+      <c r="J138" s="11"/>
+    </row>
+    <row r="139" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A139" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="B139" s="2" t="s">
         <v>762</v>
       </c>
-      <c r="C138" s="13" t="s">
+      <c r="C139" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D138" s="13" t="s">
+      <c r="D139" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="E138" s="13"/>
-      <c r="F138" s="13"/>
-      <c r="G138" s="13" t="s">
+      <c r="E139" s="13"/>
+      <c r="F139" s="13"/>
+      <c r="G139" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="H138" s="13"/>
-      <c r="I138" s="13" t="s">
+      <c r="H139" s="13"/>
+      <c r="I139" s="13" t="s">
         <v>548</v>
       </c>
-      <c r="J138" s="11"/>
-    </row>
-    <row r="139" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A139" s="12" t="s">
+      <c r="J139" s="11"/>
+    </row>
+    <row r="140" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A140" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="B140" s="2" t="s">
         <v>763</v>
       </c>
-      <c r="C139" s="13" t="s">
+      <c r="C140" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="D139" s="13" t="s">
+      <c r="D140" s="13" t="s">
         <v>421</v>
       </c>
-      <c r="E139" s="13">
+      <c r="E140" s="13">
         <v>1861</v>
       </c>
-      <c r="F139" s="13">
+      <c r="F140" s="13">
         <v>1941</v>
       </c>
-      <c r="G139" s="13" t="s">
+      <c r="G140" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="H139" t="s">
+      <c r="H140" t="s">
         <v>420</v>
       </c>
-      <c r="I139" s="13" t="s">
+      <c r="I140" s="13" t="s">
         <v>549</v>
       </c>
-      <c r="J139" s="11"/>
-    </row>
-    <row r="140" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A140" s="12" t="s">
+      <c r="J140" s="11"/>
+    </row>
+    <row r="141" spans="1:10" ht="120" x14ac:dyDescent="0.2">
+      <c r="A141" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="B141" s="2" t="s">
         <v>764</v>
-      </c>
-      <c r="C140" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D140" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="E140" s="13">
-        <v>1833</v>
-      </c>
-      <c r="F140" s="13">
-        <v>1895</v>
-      </c>
-      <c r="G140" s="13" t="s">
-        <v>922</v>
-      </c>
-      <c r="H140" t="s">
-        <v>422</v>
-      </c>
-      <c r="I140" s="13" t="s">
-        <v>468</v>
-      </c>
-      <c r="J140" s="11"/>
-    </row>
-    <row r="141" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A141" s="12" t="s">
-        <v>268</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>765</v>
       </c>
       <c r="C141" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D141" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E141" s="13">
+        <v>1833</v>
+      </c>
+      <c r="F141" s="13">
+        <v>1895</v>
+      </c>
+      <c r="G141" s="13" t="s">
+        <v>922</v>
+      </c>
+      <c r="H141" t="s">
+        <v>422</v>
+      </c>
+      <c r="I141" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="J141" s="11"/>
+    </row>
+    <row r="142" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A142" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="C142" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D142" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="E141" s="13">
+      <c r="E142" s="13">
         <v>1842</v>
       </c>
-      <c r="F141" s="13">
+      <c r="F142" s="13">
         <v>1927</v>
       </c>
-      <c r="G141" s="13" t="s">
+      <c r="G142" s="13" t="s">
         <v>923</v>
       </c>
-      <c r="H141" t="s">
+      <c r="H142" t="s">
         <v>423</v>
       </c>
-      <c r="I141" s="13" t="s">
+      <c r="I142" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="J141" s="11"/>
-    </row>
-    <row r="142" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A142" s="12" t="s">
+      <c r="J142" s="11"/>
+    </row>
+    <row r="143" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+      <c r="A143" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B143" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="C142" s="13" t="s">
+      <c r="C143" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="D142" s="13" t="s">
+      <c r="D143" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="E142" s="13">
+      <c r="E143" s="13">
         <v>1847</v>
       </c>
-      <c r="F142" s="13">
+      <c r="F143" s="13">
         <v>1916</v>
       </c>
-      <c r="G142" s="45" t="s">
+      <c r="G143" s="45" t="s">
         <v>924</v>
       </c>
-      <c r="H142" t="s">
+      <c r="H143" t="s">
         <v>424</v>
       </c>
-      <c r="I142" s="13" t="s">
+      <c r="I143" s="13" t="s">
         <v>466</v>
       </c>
-      <c r="J142" s="11"/>
-    </row>
-    <row r="143" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A143" s="12" t="s">
+      <c r="J143" s="11"/>
+    </row>
+    <row r="144" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A144" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B144" s="2" t="s">
         <v>767</v>
-      </c>
-      <c r="C143" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D143" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="E143" s="13">
-        <v>1849</v>
-      </c>
-      <c r="F143" s="13">
-        <v>1913</v>
-      </c>
-      <c r="G143" s="13" t="s">
-        <v>925</v>
-      </c>
-      <c r="H143" t="s">
-        <v>425</v>
-      </c>
-      <c r="I143" s="13" t="s">
-        <v>465</v>
-      </c>
-      <c r="J143" s="11"/>
-    </row>
-    <row r="144" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A144" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>768</v>
       </c>
       <c r="C144" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D144" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="E144" s="13">
+        <v>1849</v>
+      </c>
+      <c r="F144" s="13">
+        <v>1913</v>
+      </c>
+      <c r="G144" s="13" t="s">
+        <v>925</v>
+      </c>
+      <c r="H144" t="s">
+        <v>425</v>
+      </c>
+      <c r="I144" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="J144" s="11"/>
+    </row>
+    <row r="145" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A145" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="C145" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D145" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="E144" s="13">
+      <c r="E145" s="13">
         <v>1861</v>
       </c>
-      <c r="F144" s="13" t="s">
+      <c r="F145" s="13" t="s">
         <v>276</v>
       </c>
-      <c r="G144" s="13" t="s">
+      <c r="G145" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="H144" t="s">
+      <c r="H145" t="s">
         <v>426</v>
       </c>
-      <c r="I144" s="13" t="s">
+      <c r="I145" s="13" t="s">
         <v>550</v>
       </c>
-      <c r="J144" s="11"/>
-    </row>
-    <row r="145" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A145" s="12" t="s">
+      <c r="J145" s="11"/>
+    </row>
+    <row r="146" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A146" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B146" s="2" t="s">
         <v>769</v>
       </c>
-      <c r="C145" s="13" t="s">
+      <c r="C146" s="13" t="s">
         <v>279</v>
       </c>
-      <c r="D145" s="13" t="s">
+      <c r="D146" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="E145" s="13">
+      <c r="E146" s="13">
         <v>1847</v>
       </c>
-      <c r="F145" s="13">
+      <c r="F146" s="13">
         <v>1926</v>
       </c>
-      <c r="G145" s="13" t="s">
+      <c r="G146" s="13" t="s">
         <v>926</v>
       </c>
-      <c r="H145" t="s">
+      <c r="H146" t="s">
         <v>427</v>
       </c>
-      <c r="I145" s="13" t="s">
+      <c r="I146" s="13" t="s">
         <v>464</v>
       </c>
-      <c r="J145" s="11"/>
-    </row>
-    <row r="146" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A146" s="14" t="s">
+      <c r="J146" s="11"/>
+    </row>
+    <row r="147" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A147" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="B147" s="2" t="s">
         <v>770</v>
       </c>
-      <c r="C146" s="15" t="s">
+      <c r="C147" s="15" t="s">
         <v>281</v>
       </c>
-      <c r="D146" s="15" t="s">
+      <c r="D147" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E146" s="15">
+      <c r="E147" s="15">
         <v>1845</v>
       </c>
-      <c r="F146" s="15">
+      <c r="F147" s="15">
         <v>1921</v>
       </c>
-      <c r="G146" s="15" t="s">
+      <c r="G147" s="15" t="s">
         <v>927</v>
       </c>
-      <c r="H146" s="15"/>
-      <c r="I146" s="15" t="s">
+      <c r="H147" s="15"/>
+      <c r="I147" s="15" t="s">
         <v>463</v>
       </c>
-      <c r="J146" s="16"/>
-    </row>
-    <row r="147" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A147" s="25" t="s">
+      <c r="J147" s="16"/>
+    </row>
+    <row r="148" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="A148" s="25" t="s">
         <v>282</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="B148" s="2" t="s">
         <v>771</v>
       </c>
-      <c r="C147" s="26" t="s">
+      <c r="C148" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D147" s="26" t="s">
+      <c r="D148" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E147" s="26">
+      <c r="E148" s="26">
         <v>1855</v>
       </c>
-      <c r="F147" s="26">
+      <c r="F148" s="26">
         <v>1940</v>
       </c>
-      <c r="G147" s="26" t="s">
+      <c r="G148" s="26" t="s">
         <v>928</v>
       </c>
-      <c r="H147" t="s">
+      <c r="H148" t="s">
         <v>428</v>
       </c>
-      <c r="I147" s="27" t="s">
+      <c r="I148" s="27" t="s">
         <v>462</v>
       </c>
-      <c r="J147" s="28"/>
-    </row>
-    <row r="148" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A148" s="29" t="s">
+      <c r="J148" s="28"/>
+    </row>
+    <row r="149" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A149" s="29" t="s">
         <v>283</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="B149" s="2" t="s">
         <v>772</v>
-      </c>
-      <c r="C148" s="30"/>
-      <c r="D148" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E148" s="30">
-        <v>1846</v>
-      </c>
-      <c r="F148" s="30">
-        <v>1907</v>
-      </c>
-      <c r="G148" s="30" t="s">
-        <v>284</v>
-      </c>
-      <c r="H148" t="s">
-        <v>429</v>
-      </c>
-      <c r="I148" s="31" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="149" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A149" s="32" t="s">
-        <v>285</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>773</v>
       </c>
       <c r="C149" s="30"/>
       <c r="D149" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E149" s="30">
+        <v>1846</v>
+      </c>
+      <c r="F149" s="30">
+        <v>1907</v>
+      </c>
+      <c r="G149" s="30" t="s">
+        <v>284</v>
+      </c>
+      <c r="H149" t="s">
+        <v>429</v>
+      </c>
+      <c r="I149" s="31" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A150" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="C150" s="30"/>
+      <c r="D150" s="30" t="s">
         <v>286</v>
       </c>
-      <c r="E149" s="30">
+      <c r="E150" s="30">
         <v>1858</v>
       </c>
-      <c r="F149" s="30">
+      <c r="F150" s="30">
         <v>1940</v>
       </c>
-      <c r="G149" s="30" t="s">
+      <c r="G150" s="30" t="s">
         <v>287</v>
       </c>
-      <c r="H149" t="s">
+      <c r="H150" t="s">
         <v>430</v>
       </c>
-      <c r="I149" s="31" t="s">
+      <c r="I150" s="31" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="150" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A150" s="32" t="s">
+    <row r="151" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="A151" s="32" t="s">
         <v>288</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="B151" s="2" t="s">
         <v>774</v>
       </c>
-      <c r="C150" s="30" t="s">
+      <c r="C151" s="30" t="s">
         <v>289</v>
       </c>
-      <c r="D150" s="30" t="s">
+      <c r="D151" s="30" t="s">
         <v>290</v>
       </c>
-      <c r="E150" s="30">
+      <c r="E151" s="30">
         <v>1856</v>
       </c>
-      <c r="F150" s="30">
+      <c r="F151" s="30">
         <v>1945</v>
       </c>
-      <c r="G150" s="30" t="s">
+      <c r="G151" s="30" t="s">
         <v>929</v>
       </c>
-      <c r="H150" t="s">
+      <c r="H151" t="s">
         <v>431</v>
       </c>
-      <c r="I150" s="31" t="s">
+      <c r="I151" s="31" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A151" s="25" t="s">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A152" s="25" t="s">
         <v>433</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="B152" s="2" t="s">
         <v>775</v>
       </c>
-      <c r="C151" s="26" t="s">
+      <c r="C152" s="26" t="s">
         <v>291</v>
       </c>
-      <c r="D151" s="27" t="s">
+      <c r="D152" s="27" t="s">
         <v>432</v>
       </c>
-      <c r="E151" s="27">
+      <c r="E152" s="27">
         <v>1849</v>
       </c>
-      <c r="F151" s="27">
+      <c r="F152" s="27">
         <v>1925</v>
       </c>
-      <c r="G151" s="27" t="s">
+      <c r="G152" s="27" t="s">
         <v>930</v>
       </c>
-      <c r="H151" t="s">
+      <c r="H152" t="s">
         <v>434</v>
       </c>
-      <c r="I151" s="28" t="s">
+      <c r="I152" s="28" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="152" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A152" s="12" t="s">
+    <row r="153" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A153" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="B153" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="C152" s="13"/>
-      <c r="D152" s="13" t="s">
+      <c r="C153" s="13"/>
+      <c r="D153" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="E152" s="13">
+      <c r="E153" s="13">
         <v>1848</v>
       </c>
-      <c r="F152" s="13">
+      <c r="F153" s="13">
         <v>1921</v>
       </c>
-      <c r="G152" s="13" t="s">
+      <c r="G153" s="13" t="s">
         <v>931</v>
       </c>
-      <c r="H152" t="s">
+      <c r="H153" t="s">
         <v>435</v>
       </c>
-      <c r="I152" s="13" t="s">
+      <c r="I153" s="13" t="s">
         <v>553</v>
       </c>
-      <c r="J152" s="18"/>
-    </row>
-    <row r="153" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A153" s="12" t="s">
+      <c r="J153" s="18"/>
+    </row>
+    <row r="154" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A154" s="12" t="s">
         <v>294</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="B154" s="2" t="s">
         <v>777</v>
       </c>
-      <c r="C153" s="13" t="s">
+      <c r="C154" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D153" s="13" t="s">
+      <c r="D154" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="E153" s="13">
+      <c r="E154" s="13">
         <v>1851</v>
       </c>
-      <c r="F153" s="13">
+      <c r="F154" s="13">
         <v>1927</v>
       </c>
-      <c r="G153" s="13" t="s">
+      <c r="G154" s="13" t="s">
         <v>932</v>
       </c>
-      <c r="H153" t="s">
+      <c r="H154" t="s">
         <v>436</v>
       </c>
-      <c r="I153" s="13" t="s">
+      <c r="I154" s="13" t="s">
         <v>554</v>
       </c>
-      <c r="J153" s="11" t="s">
+      <c r="J154" s="11" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="154" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A154" s="12" t="s">
+    <row r="155" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="A155" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="B155" s="2" t="s">
         <v>778</v>
       </c>
-      <c r="C154" s="13"/>
-      <c r="D154" s="13" t="s">
+      <c r="C155" s="13"/>
+      <c r="D155" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="E154" s="13">
+      <c r="E155" s="13">
         <v>1862</v>
       </c>
-      <c r="F154" s="13">
+      <c r="F155" s="13">
         <v>1941</v>
       </c>
-      <c r="G154" s="13" t="s">
+      <c r="G155" s="13" t="s">
         <v>933</v>
       </c>
-      <c r="H154" t="s">
+      <c r="H155" t="s">
         <v>437</v>
       </c>
-      <c r="I154" s="10" t="s">
+      <c r="I155" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="J154" s="18"/>
-    </row>
-    <row r="155" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A155" s="12" t="s">
+      <c r="J155" s="18"/>
+    </row>
+    <row r="156" spans="1:10" ht="75" x14ac:dyDescent="0.2">
+      <c r="A156" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="B156" s="2" t="s">
         <v>779</v>
       </c>
-      <c r="C155" s="13" t="s">
+      <c r="C156" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D155" s="13" t="s">
+      <c r="D156" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="E155" s="13">
+      <c r="E156" s="13">
         <v>1849</v>
       </c>
-      <c r="F155" s="13">
+      <c r="F156" s="13">
         <v>1934</v>
       </c>
-      <c r="G155" s="13" t="s">
+      <c r="G156" s="13" t="s">
         <v>934</v>
       </c>
-      <c r="H155" t="s">
+      <c r="H156" t="s">
         <v>438</v>
       </c>
-      <c r="I155" s="13" t="s">
+      <c r="I156" s="13" t="s">
         <v>555</v>
       </c>
-      <c r="J155" s="11"/>
-    </row>
-    <row r="156" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A156" s="12" t="s">
+      <c r="J156" s="11"/>
+    </row>
+    <row r="157" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="A157" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="B157" s="2" t="s">
         <v>780</v>
       </c>
-      <c r="C156" s="13" t="s">
+      <c r="C157" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D156" s="13" t="s">
+      <c r="D157" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="E156" s="13">
+      <c r="E157" s="13">
         <v>1864</v>
       </c>
-      <c r="F156" s="13">
+      <c r="F157" s="13">
         <v>1937</v>
       </c>
-      <c r="G156" s="13" t="s">
+      <c r="G157" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="H156" t="s">
+      <c r="H157" t="s">
         <v>439</v>
       </c>
-      <c r="I156" s="13" t="s">
+      <c r="I157" s="13" t="s">
         <v>556</v>
       </c>
-      <c r="J156" s="11"/>
+      <c r="J157" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="H19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H18" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H20" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="H57" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="H55" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="H75" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H134" r:id="rId8" xr:uid="{CE6E5F9B-DEF9-4779-96E8-7813D6512A30}"/>
+    <hyperlink ref="H12" r:id="rId1"/>
+    <hyperlink ref="H19" r:id="rId2"/>
+    <hyperlink ref="H18" r:id="rId3"/>
+    <hyperlink ref="H20" r:id="rId4"/>
+    <hyperlink ref="H57" r:id="rId5"/>
+    <hyperlink ref="H55" r:id="rId6"/>
+    <hyperlink ref="H76" r:id="rId7"/>
+    <hyperlink ref="H135" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>

</xml_diff>